<commit_message>
Rememorando el tiempo devorado
Con un agrio sabor a NADA en la garganta
</commit_message>
<xml_diff>
--- a/Bandeja_B/Bandeja_B.xlsx
+++ b/Bandeja_B/Bandeja_B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\EUE\Practica2_EUE\Bandeja_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBF0B76-D288-4214-B8A5-ADF724BCE179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5BBEC-E1CF-4B6F-BC23-671F0290C0E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="96">
   <si>
     <t xml:space="preserve">Número de iteración </t>
   </si>
@@ -266,6 +266,84 @@
   </si>
   <si>
     <t>.030    .002    .021    .030</t>
+  </si>
+  <si>
+    <t>1x1_comp</t>
+  </si>
+  <si>
+    <t>.001     .001</t>
+  </si>
+  <si>
+    <t>.001     .002</t>
+  </si>
+  <si>
+    <t>I6_comp</t>
+  </si>
+  <si>
+    <t>.030    .002    .021    .026</t>
+  </si>
+  <si>
+    <t>I7_comp</t>
+  </si>
+  <si>
+    <t>Comp_91</t>
+  </si>
+  <si>
+    <t>I8_comp</t>
+  </si>
+  <si>
+    <t>I9_comp</t>
+  </si>
+  <si>
+    <t>.030    .002    .021    .025</t>
+  </si>
+  <si>
+    <t>.030    .001    .021    .025</t>
+  </si>
+  <si>
+    <t>I10_comp</t>
+  </si>
+  <si>
+    <t>.030    .001    .021    .026</t>
+  </si>
+  <si>
+    <t>I11_comp</t>
+  </si>
+  <si>
+    <t>I12_comp</t>
+  </si>
+  <si>
+    <t>.030    .0019  .021    .025</t>
+  </si>
+  <si>
+    <t>.030    .0018  .021    .025</t>
+  </si>
+  <si>
+    <t>I13_comp</t>
+  </si>
+  <si>
+    <t>I14_comp</t>
+  </si>
+  <si>
+    <t>.032    .0016  .021    .024</t>
+  </si>
+  <si>
+    <t>.033    .0015  .021    .024</t>
+  </si>
+  <si>
+    <t>I15_comp</t>
+  </si>
+  <si>
+    <t>Ya está puesto comp91</t>
+  </si>
+  <si>
+    <t>Hay que cambiar los offsets</t>
+  </si>
+  <si>
+    <t>Ánimo</t>
+  </si>
+  <si>
+    <t>Mirar si las tablas están bien</t>
   </si>
 </sst>
 </file>
@@ -375,7 +453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -768,35 +846,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1015,32 +1069,51 @@
     <xf numFmtId="11" fontId="0" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,39 +1154,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA72D4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1B3E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E5ECE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB17ED8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E5ECE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1188,6 +1268,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9C5BCD"/>
       <color rgb="FFB17ED8"/>
       <color rgb="FF9E5ECE"/>
       <color rgb="FFD1B3E7"/>
@@ -1197,7 +1278,6 @@
       <color rgb="FF893BC3"/>
       <color rgb="FF873AC0"/>
       <color rgb="FFC7A1D3"/>
-      <color rgb="FF83E4E9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1476,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="B1" colorId="23" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A9" colorId="23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1507,40 +1587,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="88" t="s">
+      <c r="F1" s="101"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="86" t="s">
+      <c r="I1" s="96"/>
+      <c r="J1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="83" t="s">
+      <c r="K1" s="94"/>
+      <c r="L1" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
     </row>
     <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="85"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +1719,7 @@
       <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="85" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="3">
@@ -1729,7 +1809,7 @@
       <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="86" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="9">
@@ -1789,7 +1869,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <f t="shared" ref="A5:A19" si="0">A4+1</f>
+        <f t="shared" ref="A5:A24" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1804,7 +1884,7 @@
       <c r="E5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="86" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="9">
@@ -1887,7 +1967,7 @@
       <c r="E6" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="87" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="32">
@@ -1950,7 +2030,7 @@
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="88" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3">
@@ -2014,7 +2094,7 @@
       <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="86" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="9">
@@ -2077,7 +2157,7 @@
       <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="86" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="9">
@@ -2140,7 +2220,7 @@
       <c r="E10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="87" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="32">
@@ -2203,7 +2283,7 @@
       <c r="E11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="88" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="3">
@@ -2266,7 +2346,7 @@
       <c r="E12" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="87" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="32">
@@ -2329,7 +2409,7 @@
       <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="88" t="s">
         <v>32</v>
       </c>
       <c r="G13" s="3">
@@ -2392,7 +2472,7 @@
       <c r="E14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="87" t="s">
         <v>32</v>
       </c>
       <c r="G14" s="32">
@@ -2455,7 +2535,7 @@
       <c r="E15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="86" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="9">
@@ -2497,7 +2577,7 @@
         <f t="array" aca="1" ref="R15" ca="1">INDIRECT(ADDRESS(K15+2,24))/(MAX(N15,O15,P15)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>9.519602622010952</v>
       </c>
-      <c r="S15" s="98">
+      <c r="S15" s="76">
         <v>14.678739999999999</v>
       </c>
     </row>
@@ -2518,7 +2598,7 @@
       <c r="E16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="86" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="9">
@@ -2581,7 +2661,7 @@
       <c r="E17" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="69" t="s">
+      <c r="F17" s="89" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="69">
@@ -2600,10 +2680,10 @@
       <c r="K17" s="72">
         <v>2</v>
       </c>
-      <c r="L17" s="96">
+      <c r="L17" s="75">
         <v>143.9923</v>
       </c>
-      <c r="M17" s="96">
+      <c r="M17" s="75">
         <v>805.81730000000005</v>
       </c>
       <c r="N17" s="73">
@@ -2615,20 +2695,20 @@
       <c r="P17" s="73">
         <v>46500000</v>
       </c>
-      <c r="Q17" s="99" cm="1">
+      <c r="Q17" s="77" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">INDIRECT(ADDRESS(K17+2,23))/(MAX(N17,O17,P17)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
         <v>1.0196634432838105</v>
       </c>
-      <c r="R17" s="99" cm="1">
+      <c r="R17" s="77" cm="1">
         <f t="array" aca="1" ref="R17" ca="1">INDIRECT(ADDRESS(K17+2,24))/(MAX(N17,O17,P17)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.89579075209573711</v>
       </c>
-      <c r="S17" s="100">
+      <c r="S17" s="78">
         <v>13.57723</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="82">
+    <row r="18" spans="1:19" s="80" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="74">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2644,7 +2724,7 @@
       <c r="E18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="86" t="s">
         <v>69</v>
       </c>
       <c r="G18" s="9">
@@ -2686,117 +2766,589 @@
         <f t="array" aca="1" ref="R18" ca="1">INDIRECT(ADDRESS(K18+2,24))/(MAX(N18,O18,P18)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.64160651717787309</v>
       </c>
-      <c r="S18" s="101">
+      <c r="S18" s="79">
         <v>17.217079999999999</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="74">
+      <c r="A19" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="76">
+      <c r="D19" s="30">
         <v>1.5200000000000001E-3</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="104" t="s">
+      <c r="F19" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="104">
-        <v>1.3299999999999999E-2</v>
-      </c>
-      <c r="H19" s="78" t="s">
+      <c r="G19" s="32">
+        <v>1.252E-2</v>
+      </c>
+      <c r="H19" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="I19" s="78">
+      <c r="I19" s="33">
         <v>1.0399999999999999E-3</v>
       </c>
-      <c r="J19" s="79" t="str" cm="1">
+      <c r="J19" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT(ADDRESS(K19+2,22))</f>
         <v>CFRP</v>
       </c>
-      <c r="K19" s="80">
+      <c r="K19" s="40">
         <v>2</v>
       </c>
-      <c r="L19" s="97">
+      <c r="L19" s="49">
         <v>141.88290000000001</v>
       </c>
-      <c r="M19" s="97">
+      <c r="M19" s="49">
         <v>787.99739999999997</v>
       </c>
-      <c r="N19" s="81">
+      <c r="N19" s="45">
         <v>10700000</v>
       </c>
-      <c r="O19" s="81">
+      <c r="O19" s="45">
         <v>7270000</v>
       </c>
-      <c r="P19" s="81">
+      <c r="P19" s="45">
         <v>86800000</v>
       </c>
-      <c r="Q19" s="102" cm="1">
+      <c r="Q19" s="46" cm="1">
         <f t="array" aca="1" ref="Q19" ca="1">INDIRECT(ADDRESS(K19+2,23))/(MAX(N19,O19,P19)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
         <v>8.1962558902041405E-2</v>
       </c>
-      <c r="R19" s="102" cm="1">
+      <c r="R19" s="46" cm="1">
         <f t="array" aca="1" ref="R19" ca="1">INDIRECT(ADDRESS(K19+2,24))/(MAX(N19,O19,P19)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.5602188622716229E-2</v>
       </c>
-      <c r="S19" s="103">
+      <c r="S19" s="52">
         <v>13.33296</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="K20" s="23"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="48"/>
+      <c r="A20" s="81">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1.3520000000000001E-2</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1.0399999999999999E-3</v>
+      </c>
+      <c r="J20" s="20" t="str" cm="1">
+        <f t="array" aca="1" ref="J20" ca="1">INDIRECT(ADDRESS(K20+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K20" s="39">
+        <v>2</v>
+      </c>
+      <c r="L20" s="18">
+        <v>162.56610000000001</v>
+      </c>
+      <c r="M20" s="18">
+        <v>818.37549999999999</v>
+      </c>
+      <c r="N20" s="18">
+        <v>7880000</v>
+      </c>
+      <c r="O20" s="18">
+        <v>7620000</v>
+      </c>
+      <c r="P20" s="18">
+        <v>33000000</v>
+      </c>
+      <c r="Q20" s="42" cm="1">
+        <f t="array" aca="1" ref="Q20" ca="1">INDIRECT(ADDRESS(K20+2,23))/(MAX(N20,O20,P20)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>1.8458893973544606</v>
+      </c>
+      <c r="R20" s="42" cm="1">
+        <f t="array" aca="1" ref="R20" ca="1">INDIRECT(ADDRESS(K20+2,24))/(MAX(N20,O20,P20)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>1.6713415143167207</v>
+      </c>
+      <c r="S20" s="82">
+        <v>14.56298</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-      <c r="K21" s="23"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="48"/>
+      <c r="A21" s="74">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.3455E-2</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J21" s="20" t="str" cm="1">
+        <f t="array" aca="1" ref="J21" ca="1">INDIRECT(ADDRESS(K21+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K21" s="39">
+        <v>2</v>
+      </c>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="83" t="e" cm="1">
+        <f t="array" aca="1" ref="Q21" ca="1">INDIRECT(ADDRESS(K21+2,23))/(MAX(N21,O21,P21)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" s="83" t="e" cm="1">
+        <f t="array" aca="1" ref="R21" ca="1">INDIRECT(ADDRESS(K21+2,24))/(MAX(N21,O21,P21)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="48"/>
+      <c r="A22" s="74">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="9">
+        <v>1.2455000000000001E-2</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J22" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J22" ca="1">INDIRECT(ADDRESS(K22+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K22" s="11">
+        <v>2</v>
+      </c>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q22" ca="1">INDIRECT(ADDRESS(K22+2,23))/(MAX(N22,O22,P22)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R22" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="R22" ca="1">INDIRECT(ADDRESS(K22+2,24))/(MAX(N22,O22,P22)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" s="43"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="48"/>
+      <c r="A23" s="74">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.2955E-2</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J23" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J23" ca="1">INDIRECT(ADDRESS(K23+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K23" s="11">
+        <v>2</v>
+      </c>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q23" ca="1">INDIRECT(ADDRESS(K23+2,23))/(MAX(N23,O23,P23)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="R23" ca="1">INDIRECT(ADDRESS(K23+2,24))/(MAX(N23,O23,P23)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" s="43"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
+      <c r="A24" s="74">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1.2955E-2</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J24" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J24" ca="1">INDIRECT(ADDRESS(K24+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K24" s="11">
+        <v>2</v>
+      </c>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q24" ca="1">INDIRECT(ADDRESS(K24+2,23))/(MAX(N24,O24,P24)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R24" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="R24" ca="1">INDIRECT(ADDRESS(K24+2,24))/(MAX(N24,O24,P24)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S24" s="84"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
+      <c r="A25" s="74">
+        <f>A24+1</f>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.3455E-2</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J25" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J25" ca="1">INDIRECT(ADDRESS(K25+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K25" s="11">
+        <v>2</v>
+      </c>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q25" ca="1">INDIRECT(ADDRESS(K25+2,23))/(MAX(N25,O25,P25)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R25" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="R25" ca="1">INDIRECT(ADDRESS(K25+2,24))/(MAX(N25,O25,P25)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S25" s="84"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
+      <c r="A26" s="74">
+        <f>A25+1</f>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.2955E-2</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J26" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J26" ca="1">INDIRECT(ADDRESS(K26+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K26" s="11">
+        <v>2</v>
+      </c>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q26" ca="1">INDIRECT(ADDRESS(K26+2,23))/(MAX(N26,O26,P26)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R26" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="R26" ca="1">INDIRECT(ADDRESS(K26+2,24))/(MAX(N26,O26,P26)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S26" s="84"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
+      <c r="A27" s="74">
+        <f>A26+1</f>
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1.2955E-2</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J27" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J27" ca="1">INDIRECT(ADDRESS(K27+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K27" s="11">
+        <v>2</v>
+      </c>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q27" ca="1">INDIRECT(ADDRESS(K27+2,23))/(MAX(N27,O27,P27)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R27" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="R27" ca="1">INDIRECT(ADDRESS(K27+2,24))/(MAX(N27,O27,P27)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S27" s="84"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B28" s="8"/>
+      <c r="A28" s="74">
+        <f>A27+1</f>
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1.2455000000000001E-2</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J28" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J28" ca="1">INDIRECT(ADDRESS(K28+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K28" s="11">
+        <v>2</v>
+      </c>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="Q28" ca="1">INDIRECT(ADDRESS(K28+2,23))/(MAX(N28,O28,P28)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R28" s="22" t="e" cm="1">
+        <f t="array" aca="1" ref="R28" ca="1">INDIRECT(ADDRESS(K28+2,24))/(MAX(N28,O28,P28)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S28" s="84"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="8"/>
+      <c r="A29" s="74">
+        <f>A28+1</f>
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9.5500000000000001E-4</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="9">
+        <v>1.2455000000000001E-2</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J29" s="23" t="str" cm="1">
+        <f t="array" aca="1" ref="J29" ca="1">INDIRECT(ADDRESS(K29+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K29" s="11">
+        <v>2</v>
+      </c>
+      <c r="S29" s="84"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
@@ -2837,23 +3389,34 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:L18 L20:L1048576">
+  <conditionalFormatting sqref="L3:L18 L21:L1048576">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+      <formula>150</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S18 S21:S1048576">
+    <cfRule type="top10" dxfId="13" priority="11" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="12" priority="12" percent="1" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="11" priority="13" rank="4"/>
+    <cfRule type="top10" dxfId="10" priority="14" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S18 S20:S1048576">
+  <conditionalFormatting sqref="S19">
     <cfRule type="top10" dxfId="8" priority="6" bottom="1" rank="4"/>
     <cfRule type="top10" dxfId="7" priority="7" percent="1" bottom="1" rank="4"/>
     <cfRule type="top10" dxfId="6" priority="8" rank="4"/>
     <cfRule type="top10" dxfId="5" priority="9" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
+  <conditionalFormatting sqref="L20">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S19">
+  <conditionalFormatting sqref="S20">
     <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="4"/>
     <cfRule type="top10" dxfId="2" priority="2" percent="1" bottom="1" rank="4"/>
     <cfRule type="top10" dxfId="1" priority="3" rank="4"/>

</xml_diff>

<commit_message>
Imagenes para el informe
</commit_message>
<xml_diff>
--- a/Bandeja_B/Bandeja_B.xlsx
+++ b/Bandeja_B/Bandeja_B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\EUE\Practica2_EUE\Bandeja_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A3A893-B8E2-403F-A71E-5BE130EF029F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD5796-5EAB-4361-8ED0-92DF1E2986B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -910,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,13 +1151,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1213,6 +1207,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,6 +1330,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF9C5BCD"/>
       <color rgb="FFB17ED8"/>
@@ -1614,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD41"/>
+  <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="F19" colorId="23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="G16" colorId="23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,40 +1716,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="101"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="95" t="s">
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="93" t="s">
+      <c r="I1" s="94"/>
+      <c r="J1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="90" t="s">
+      <c r="K1" s="92"/>
+      <c r="L1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
     </row>
     <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="92"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
@@ -1779,7 +1848,7 @@
       <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="83" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="3">
@@ -1869,7 +1938,7 @@
       <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="84" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="9">
@@ -1944,7 +2013,7 @@
       <c r="E5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="84" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="9">
@@ -2027,7 +2096,7 @@
       <c r="E6" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="85" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="32">
@@ -2090,7 +2159,7 @@
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="88" t="s">
+      <c r="F7" s="86" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="3">
@@ -2154,7 +2223,7 @@
       <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="84" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="9">
@@ -2217,7 +2286,7 @@
       <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="84" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="9">
@@ -2249,15 +2318,15 @@
         <v>7870000</v>
       </c>
       <c r="P9" s="43">
-        <v>3840000</v>
+        <v>38400000</v>
       </c>
       <c r="Q9" s="44" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">INDIRECT(ADDRESS(K9+2,23))/(MAX(N9,O9,P9)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
-        <v>39.016025503334767</v>
+        <v>7.2012010601886622</v>
       </c>
       <c r="R9" s="44" cm="1">
         <f t="array" aca="1" ref="R9" ca="1">INDIRECT(ADDRESS(K9+2,24))/(MAX(N9,O9,P9)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
-        <v>39.044665203496209</v>
+        <v>7.2070707070707059</v>
       </c>
       <c r="S9" s="54">
         <v>17.30743</v>
@@ -2280,7 +2349,7 @@
       <c r="E10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="87" t="s">
+      <c r="F10" s="85" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="32">
@@ -2343,7 +2412,7 @@
       <c r="E11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="86" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="3">
@@ -2406,7 +2475,7 @@
       <c r="E12" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="87" t="s">
+      <c r="F12" s="85" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="32">
@@ -2469,7 +2538,7 @@
       <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="86" t="s">
         <v>32</v>
       </c>
       <c r="G13" s="3">
@@ -2532,7 +2601,7 @@
       <c r="E14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="87" t="s">
+      <c r="F14" s="85" t="s">
         <v>32</v>
       </c>
       <c r="G14" s="32">
@@ -2595,7 +2664,7 @@
       <c r="E15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="86" t="s">
+      <c r="F15" s="84" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="9">
@@ -2658,7 +2727,7 @@
       <c r="E16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="86" t="s">
+      <c r="F16" s="84" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="9">
@@ -2721,7 +2790,7 @@
       <c r="E17" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="89" t="s">
+      <c r="F17" s="87" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="69">
@@ -2784,7 +2853,7 @@
       <c r="E18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="86" t="s">
+      <c r="F18" s="84" t="s">
         <v>69</v>
       </c>
       <c r="G18" s="9">
@@ -2847,7 +2916,7 @@
       <c r="E19" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="87" t="s">
+      <c r="F19" s="85" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="32">
@@ -2910,7 +2979,7 @@
       <c r="E20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="88" t="s">
+      <c r="F20" s="86" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="3">
@@ -2929,10 +2998,10 @@
       <c r="K20" s="39">
         <v>2</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="50">
         <v>162.56610000000001</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="50">
         <v>818.37549999999999</v>
       </c>
       <c r="N20" s="18">
@@ -2952,7 +3021,7 @@
         <f t="array" aca="1" ref="R20" ca="1">INDIRECT(ADDRESS(K20+2,24))/(MAX(N20,O20,P20)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.6713415143167207</v>
       </c>
-      <c r="S20" s="82">
+      <c r="S20" s="102">
         <v>14.56298</v>
       </c>
     </row>
@@ -2973,7 +3042,7 @@
       <c r="E21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="88" t="s">
+      <c r="F21" s="86" t="s">
         <v>74</v>
       </c>
       <c r="G21" s="3">
@@ -2992,10 +3061,10 @@
       <c r="K21" s="39">
         <v>2</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="50">
         <v>161.84139999999999</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="50">
         <v>815.18520000000001</v>
       </c>
       <c r="N21" s="18">
@@ -3007,15 +3076,15 @@
       <c r="P21" s="18">
         <v>33900000</v>
       </c>
-      <c r="Q21" s="83" cm="1">
+      <c r="Q21" s="82" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">INDIRECT(ADDRESS(K21+2,23))/(MAX(N21,O21,P21)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
         <v>1.7703348115839881</v>
       </c>
-      <c r="R21" s="83" cm="1">
+      <c r="R21" s="82" cm="1">
         <f t="array" aca="1" ref="R21" ca="1">INDIRECT(ADDRESS(K21+2,24))/(MAX(N21,O21,P21)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.6004209431401706</v>
       </c>
-      <c r="S21" s="18">
+      <c r="S21" s="50">
         <v>14.48343</v>
       </c>
     </row>
@@ -3036,7 +3105,7 @@
       <c r="E22" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="86" t="s">
+      <c r="F22" s="84" t="s">
         <v>33</v>
       </c>
       <c r="G22" s="9">
@@ -3055,10 +3124,10 @@
       <c r="K22" s="11">
         <v>2</v>
       </c>
-      <c r="L22" s="43">
+      <c r="L22" s="48">
         <v>139.0222</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M22" s="48">
         <v>782.95159999999998</v>
       </c>
       <c r="N22" s="43">
@@ -3078,7 +3147,7 @@
         <f t="array" aca="1" ref="R22" ca="1">INDIRECT(ADDRESS(K22+2,24))/(MAX(N22,O22,P22)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.77016606370385099</v>
       </c>
-      <c r="S22" s="43">
+      <c r="S22" s="48">
         <v>13.24066</v>
       </c>
     </row>
@@ -3099,7 +3168,7 @@
       <c r="E23" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="86" t="s">
+      <c r="F23" s="84" t="s">
         <v>79</v>
       </c>
       <c r="G23" s="3">
@@ -3118,10 +3187,10 @@
       <c r="K23" s="11">
         <v>2</v>
       </c>
-      <c r="L23" s="43">
+      <c r="L23" s="48">
         <v>151.31309999999999</v>
       </c>
-      <c r="M23" s="43">
+      <c r="M23" s="48">
         <v>803.09820000000002</v>
       </c>
       <c r="N23" s="43">
@@ -3141,7 +3210,7 @@
         <f t="array" aca="1" ref="R23" ca="1">INDIRECT(ADDRESS(K23+2,24))/(MAX(N23,O23,P23)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1928922878719348</v>
       </c>
-      <c r="S23" s="43">
+      <c r="S23" s="48">
         <v>13.86205</v>
       </c>
     </row>
@@ -3162,7 +3231,7 @@
       <c r="E24" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="86" t="s">
+      <c r="F24" s="84" t="s">
         <v>80</v>
       </c>
       <c r="G24" s="3">
@@ -3181,10 +3250,10 @@
       <c r="K24" s="11">
         <v>2</v>
       </c>
-      <c r="L24" s="43">
+      <c r="L24" s="48">
         <v>126.6069</v>
       </c>
-      <c r="M24" s="43">
+      <c r="M24" s="48">
         <v>742.78200000000004</v>
       </c>
       <c r="N24" s="43">
@@ -3204,13 +3273,13 @@
         <f t="array" aca="1" ref="R24" ca="1">INDIRECT(ADDRESS(K24+2,24))/(MAX(N24,O24,P24)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1553611240208257</v>
       </c>
-      <c r="S24" s="84">
+      <c r="S24" s="103">
         <v>13.37659</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="74">
-        <f>A24+1</f>
+        <f t="shared" ref="A25:A31" si="1">A24+1</f>
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3225,7 +3294,7 @@
       <c r="E25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="88" t="s">
+      <c r="F25" s="86" t="s">
         <v>82</v>
       </c>
       <c r="G25" s="3">
@@ -3244,10 +3313,10 @@
       <c r="K25" s="11">
         <v>2</v>
       </c>
-      <c r="L25" s="43">
+      <c r="L25" s="48">
         <v>134.1542</v>
       </c>
-      <c r="M25" s="43">
+      <c r="M25" s="48">
         <v>739.21569999999997</v>
       </c>
       <c r="N25" s="43">
@@ -3267,13 +3336,13 @@
         <f t="array" aca="1" ref="R25" ca="1">INDIRECT(ADDRESS(K25+2,24))/(MAX(N25,O25,P25)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.5700953344738129</v>
       </c>
-      <c r="S25" s="84">
+      <c r="S25" s="103">
         <v>13.97856</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="74">
-        <f>A25+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3288,7 +3357,7 @@
       <c r="E26" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="86" t="s">
+      <c r="F26" s="84" t="s">
         <v>86</v>
       </c>
       <c r="G26" s="3">
@@ -3307,10 +3376,10 @@
       <c r="K26" s="11">
         <v>2</v>
       </c>
-      <c r="L26" s="43">
+      <c r="L26" s="48">
         <v>147.46780000000001</v>
       </c>
-      <c r="M26" s="43">
+      <c r="M26" s="48">
         <v>795.86620000000005</v>
       </c>
       <c r="N26" s="43">
@@ -3330,13 +3399,13 @@
         <f t="array" aca="1" ref="R26" ca="1">INDIRECT(ADDRESS(K26+2,24))/(MAX(N26,O26,P26)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1820363854567271</v>
       </c>
-      <c r="S26" s="84">
+      <c r="S26" s="103">
         <v>13.76496</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="74">
-        <f>A26+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3351,7 +3420,7 @@
       <c r="E27" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="86" t="s">
+      <c r="F27" s="84" t="s">
         <v>85</v>
       </c>
       <c r="G27" s="3">
@@ -3370,10 +3439,10 @@
       <c r="K27" s="11">
         <v>2</v>
       </c>
-      <c r="L27" s="43">
+      <c r="L27" s="48">
         <v>149.43559999999999</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="48">
         <v>799.65239999999994</v>
       </c>
       <c r="N27" s="43">
@@ -3393,13 +3462,13 @@
         <f t="array" aca="1" ref="R27" ca="1">INDIRECT(ADDRESS(K27+2,24))/(MAX(N27,O27,P27)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1874508678027733</v>
       </c>
-      <c r="S27" s="84">
+      <c r="S27" s="103">
         <v>13.813499999999999</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="74">
-        <f>A27+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3414,7 +3483,7 @@
       <c r="E28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="86" t="s">
+      <c r="F28" s="84" t="s">
         <v>89</v>
       </c>
       <c r="G28" s="9">
@@ -3433,10 +3502,10 @@
       <c r="K28" s="11">
         <v>2</v>
       </c>
-      <c r="L28" s="43">
+      <c r="L28" s="48">
         <v>132.9813</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="48">
         <v>771.09990000000005</v>
       </c>
       <c r="N28" s="43">
@@ -3456,13 +3525,13 @@
         <f t="array" aca="1" ref="R28" ca="1">INDIRECT(ADDRESS(K28+2,24))/(MAX(N28,O28,P28)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.95464013242686852</v>
       </c>
-      <c r="S28" s="84">
+      <c r="S28" s="103">
         <v>13.17076</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="74">
-        <f>A28+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3477,7 +3546,7 @@
       <c r="E29" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="86" t="s">
+      <c r="F29" s="84" t="s">
         <v>90</v>
       </c>
       <c r="G29" s="9">
@@ -3496,10 +3565,10 @@
       <c r="K29" s="11">
         <v>2</v>
       </c>
-      <c r="L29" s="43">
+      <c r="L29" s="48">
         <v>131.4419</v>
       </c>
-      <c r="M29" s="43">
+      <c r="M29" s="48">
         <v>766.68520000000001</v>
       </c>
       <c r="N29" s="43">
@@ -3519,13 +3588,13 @@
         <f t="array" aca="1" ref="R29" ca="1">INDIRECT(ADDRESS(K29+2,24))/(MAX(N29,O29,P29)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.86767521128075797</v>
       </c>
-      <c r="S29" s="84">
+      <c r="S29" s="103">
         <v>13.182410000000001</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="74">
-        <f>A29+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3540,7 +3609,7 @@
       <c r="E30" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="86" t="s">
+      <c r="F30" s="84" t="s">
         <v>93</v>
       </c>
       <c r="G30" s="3">
@@ -3559,10 +3628,10 @@
       <c r="K30" s="11">
         <v>2</v>
       </c>
-      <c r="L30" s="43">
+      <c r="L30" s="48">
         <v>119.8836</v>
       </c>
-      <c r="M30" s="43">
+      <c r="M30" s="48">
         <v>717.33270000000005</v>
       </c>
       <c r="N30" s="43">
@@ -3582,13 +3651,13 @@
         <f t="array" aca="1" ref="R30" ca="1">INDIRECT(ADDRESS(K30+2,24))/(MAX(N30,O30,P30)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.2778881129832498</v>
       </c>
-      <c r="S30" s="84">
+      <c r="S30" s="103">
         <v>13.37659</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="74">
-        <f>A30+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3603,7 +3672,7 @@
       <c r="E31" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="88" t="s">
+      <c r="F31" s="86" t="s">
         <v>95</v>
       </c>
       <c r="G31" s="3">
@@ -3622,10 +3691,10 @@
       <c r="K31" s="11">
         <v>2</v>
       </c>
-      <c r="L31" s="43">
+      <c r="L31" s="48">
         <v>121.24299999999999</v>
       </c>
-      <c r="M31" s="43">
+      <c r="M31" s="48">
         <v>740.49220000000003</v>
       </c>
       <c r="N31" s="43">
@@ -3645,13 +3714,13 @@
         <f t="array" aca="1" ref="R31" ca="1">INDIRECT(ADDRESS(K31+2,24))/(MAX(N31,O31,P31)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.27023443764339738</v>
       </c>
-      <c r="S31" s="84">
+      <c r="S31" s="103">
         <v>11.9008</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="74">
-        <f t="shared" ref="A32:A41" si="1">A31+1</f>
+        <f t="shared" ref="A32:A41" si="2">A31+1</f>
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3666,7 +3735,7 @@
       <c r="E32" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="88" t="s">
+      <c r="F32" s="86" t="s">
         <v>97</v>
       </c>
       <c r="G32" s="3">
@@ -3685,10 +3754,10 @@
       <c r="K32" s="11">
         <v>2</v>
       </c>
-      <c r="L32" s="43">
+      <c r="L32" s="48">
         <v>123.3674</v>
       </c>
-      <c r="M32" s="43">
+      <c r="M32" s="48">
         <v>749.61800000000005</v>
       </c>
       <c r="N32" s="43">
@@ -3708,13 +3777,13 @@
         <f t="array" aca="1" ref="R32" ca="1">INDIRECT(ADDRESS(K32+2,24))/(MAX(N32,O32,P32)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.34176971038739401</v>
       </c>
-      <c r="S32" s="84">
+      <c r="S32" s="103">
         <v>11.9979</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3729,7 +3798,7 @@
       <c r="E33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="88" t="s">
+      <c r="F33" s="86" t="s">
         <v>98</v>
       </c>
       <c r="G33" s="3">
@@ -3748,10 +3817,10 @@
       <c r="K33" s="11">
         <v>2</v>
       </c>
-      <c r="L33" s="43">
+      <c r="L33" s="48">
         <v>132.3115</v>
       </c>
-      <c r="M33" s="43">
+      <c r="M33" s="48">
         <v>770.77909999999997</v>
       </c>
       <c r="N33" s="43">
@@ -3771,13 +3840,13 @@
         <f t="array" aca="1" ref="R33" ca="1">INDIRECT(ADDRESS(K33+2,24))/(MAX(N33,O33,P33)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.53311773865133549</v>
       </c>
-      <c r="S33" s="84">
+      <c r="S33" s="103">
         <v>12.13382</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3792,7 +3861,7 @@
       <c r="E34" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="88" t="s">
+      <c r="F34" s="86" t="s">
         <v>100</v>
       </c>
       <c r="G34" s="3">
@@ -3811,10 +3880,10 @@
       <c r="K34" s="39">
         <v>2</v>
       </c>
-      <c r="L34" s="43">
+      <c r="L34" s="48">
         <v>139.16829999999999</v>
       </c>
-      <c r="M34" s="43">
+      <c r="M34" s="48">
         <v>782.17420000000004</v>
       </c>
       <c r="N34" s="43">
@@ -3834,13 +3903,13 @@
         <f t="array" aca="1" ref="R34" ca="1">INDIRECT(ADDRESS(K34+2,24))/(MAX(N34,O34,P34)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.6570351498581164</v>
       </c>
-      <c r="S34" s="84">
+      <c r="S34" s="103">
         <v>12.17266</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3855,7 +3924,7 @@
       <c r="E35" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F35" s="88" t="s">
+      <c r="F35" s="86" t="s">
         <v>103</v>
       </c>
       <c r="G35" s="3">
@@ -3874,10 +3943,10 @@
       <c r="K35" s="39">
         <v>2</v>
       </c>
-      <c r="L35" s="43">
+      <c r="L35" s="48">
         <v>143.09630000000001</v>
       </c>
-      <c r="M35" s="43">
+      <c r="M35" s="48">
         <v>795.80020000000002</v>
       </c>
       <c r="N35" s="43">
@@ -3897,13 +3966,13 @@
         <f t="array" aca="1" ref="R35" ca="1">INDIRECT(ADDRESS(K35+2,24))/(MAX(N35,O35,P35)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.87562276537131445</v>
       </c>
-      <c r="S35" s="84">
+      <c r="S35" s="103">
         <v>12.24062</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3918,7 +3987,7 @@
       <c r="E36" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F36" s="88" t="s">
+      <c r="F36" s="86" t="s">
         <v>105</v>
       </c>
       <c r="G36" s="3">
@@ -3937,10 +4006,10 @@
       <c r="K36" s="39">
         <v>2</v>
       </c>
-      <c r="L36" s="43">
+      <c r="L36" s="48">
         <v>152.0932</v>
       </c>
-      <c r="M36" s="43">
+      <c r="M36" s="48">
         <v>775.52440000000001</v>
       </c>
       <c r="N36" s="43">
@@ -3960,13 +4029,13 @@
         <f t="array" aca="1" ref="R36" ca="1">INDIRECT(ADDRESS(K36+2,24))/(MAX(N36,O36,P36)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.94172400820378366</v>
       </c>
-      <c r="S36" s="84">
+      <c r="S36" s="103">
         <v>11.990130000000001</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3981,7 +4050,7 @@
       <c r="E37" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="88" t="s">
+      <c r="F37" s="86" t="s">
         <v>107</v>
       </c>
       <c r="G37" s="3">
@@ -4000,10 +4069,10 @@
       <c r="K37" s="39">
         <v>2</v>
       </c>
-      <c r="L37" s="43">
+      <c r="L37" s="48">
         <v>157.42330000000001</v>
       </c>
-      <c r="M37" s="43">
+      <c r="M37" s="48">
         <v>771.28420000000006</v>
       </c>
       <c r="N37" s="43">
@@ -4023,13 +4092,13 @@
         <f t="array" aca="1" ref="R37" ca="1">INDIRECT(ADDRESS(K37+2,24))/(MAX(N37,O37,P37)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.95031570735512783</v>
       </c>
-      <c r="S37" s="84">
+      <c r="S37" s="103">
         <v>11.939640000000001</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -4044,7 +4113,7 @@
       <c r="E38" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="88" t="s">
+      <c r="F38" s="86" t="s">
         <v>109</v>
       </c>
       <c r="G38" s="3">
@@ -4063,10 +4132,10 @@
       <c r="K38" s="39">
         <v>2</v>
       </c>
-      <c r="L38" s="43">
+      <c r="L38" s="48">
         <v>155.74299999999999</v>
       </c>
-      <c r="M38" s="43">
+      <c r="M38" s="48">
         <v>761.43579999999997</v>
       </c>
       <c r="N38" s="43">
@@ -4086,13 +4155,13 @@
         <f t="array" aca="1" ref="R38" ca="1">INDIRECT(ADDRESS(K38+2,24))/(MAX(N38,O38,P38)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.85979472515721045</v>
       </c>
-      <c r="S38" s="84">
+      <c r="S38" s="103">
         <v>11.87168</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -4107,7 +4176,7 @@
       <c r="E39" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F39" s="88" t="s">
+      <c r="F39" s="86" t="s">
         <v>110</v>
       </c>
       <c r="G39" s="3">
@@ -4126,10 +4195,10 @@
       <c r="K39" s="39">
         <v>2</v>
       </c>
-      <c r="L39" s="43">
+      <c r="L39" s="48">
         <v>154.4623</v>
       </c>
-      <c r="M39" s="43">
+      <c r="M39" s="48">
         <v>754.29610000000002</v>
       </c>
       <c r="N39" s="43">
@@ -4149,13 +4218,13 @@
         <f t="array" aca="1" ref="R39" ca="1">INDIRECT(ADDRESS(K39+2,24))/(MAX(N39,O39,P39)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.79540264709677744</v>
       </c>
-      <c r="S39" s="84">
+      <c r="S39" s="103">
         <v>11.82799</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -4170,7 +4239,7 @@
       <c r="E40" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="88" t="s">
+      <c r="F40" s="86" t="s">
         <v>113</v>
       </c>
       <c r="G40" s="3">
@@ -4189,10 +4258,10 @@
       <c r="K40" s="39">
         <v>2</v>
       </c>
-      <c r="L40" s="43">
+      <c r="L40" s="48">
         <v>153.0994</v>
       </c>
-      <c r="M40" s="43">
+      <c r="M40" s="48">
         <v>746.97760000000005</v>
       </c>
       <c r="N40" s="43">
@@ -4212,13 +4281,13 @@
         <f t="array" aca="1" ref="R40" ca="1">INDIRECT(ADDRESS(K40+2,24))/(MAX(N40,O40,P40)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.72851509749905463</v>
       </c>
-      <c r="S40" s="84">
+      <c r="S40" s="103">
         <v>11.78429</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4233,11 +4302,11 @@
       <c r="E41" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="88" t="s">
+      <c r="F41" s="86" t="s">
         <v>115</v>
       </c>
       <c r="G41" s="3">
-        <v>2.2655000000000002E-2</v>
+        <v>2.2955E-2</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>76</v>
@@ -4252,31 +4321,36 @@
       <c r="K41" s="39">
         <v>2</v>
       </c>
-      <c r="L41" s="43">
-        <v>151.6438</v>
-      </c>
-      <c r="M41" s="43">
-        <v>739.46709999999996</v>
+      <c r="L41" s="48">
+        <v>152.08109999999999</v>
+      </c>
+      <c r="M41" s="48">
+        <v>737.20090000000005</v>
       </c>
       <c r="N41" s="43">
-        <v>23300000</v>
+        <v>23400000</v>
       </c>
       <c r="O41" s="43">
-        <v>21800000</v>
+        <v>21900000</v>
       </c>
       <c r="P41" s="43">
-        <v>59000000</v>
+        <v>58200000</v>
       </c>
       <c r="Q41" s="21" cm="1">
         <f t="array" aca="1" ref="Q41" ca="1">INDIRECT(ADDRESS(K41+2,23))/(MAX(N41,O41,P41)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
-        <v>0.59176864597791878</v>
+        <v>0.6136486273659314</v>
       </c>
       <c r="R41" s="22" cm="1">
         <f t="array" aca="1" ref="R41" ca="1">INDIRECT(ADDRESS(K41+2,24))/(MAX(N41,O41,P41)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
-        <v>0.49414016902460656</v>
-      </c>
-      <c r="S41" s="84">
+        <v>0.51467817822082118</v>
+      </c>
+      <c r="S41" s="103">
         <v>11.740600000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C45" s="101">
+        <v>9.5500000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificación de rigidizadores exteriores
Los resultados siguen estado dentro de los límites
</commit_message>
<xml_diff>
--- a/Bandeja_B/Bandeja_B.xlsx
+++ b/Bandeja_B/Bandeja_B.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\EUE\Practica2_EUE\Bandeja_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD5796-5EAB-4361-8ED0-92DF1E2986B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE83657-6816-4243-88DC-ADCB00A9B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="119">
   <si>
     <t xml:space="preserve">Número de iteración </t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>.0055  .0008  .0405  .045</t>
+  </si>
+  <si>
+    <t>.001     .045</t>
+  </si>
+  <si>
+    <t>1x2_comp</t>
+  </si>
+  <si>
+    <t>1x45_comp</t>
   </si>
 </sst>
 </file>
@@ -1169,6 +1178,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1207,21 +1225,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA72D4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1B3E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E5ECE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB17ED8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1289,34 +1326,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF9E5ECE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAA72D4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD1B3E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9E5ECE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB17ED8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1428,7 +1437,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C8C8C8"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1685,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="G16" colorId="23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A25" colorId="23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,40 +1725,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="98" t="s">
+      <c r="C1" s="99"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="99"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="93" t="s">
+      <c r="F1" s="102"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="91" t="s">
+      <c r="I1" s="97"/>
+      <c r="J1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="92"/>
-      <c r="L1" s="88" t="s">
+      <c r="K1" s="95"/>
+      <c r="L1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
     </row>
     <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="90"/>
+      <c r="A2" s="93"/>
       <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>72</v>
@@ -3021,7 +3030,7 @@
         <f t="array" aca="1" ref="R20" ca="1">INDIRECT(ADDRESS(K20+2,24))/(MAX(N20,O20,P20)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.6713415143167207</v>
       </c>
-      <c r="S20" s="102">
+      <c r="S20" s="89">
         <v>14.56298</v>
       </c>
     </row>
@@ -3273,7 +3282,7 @@
         <f t="array" aca="1" ref="R24" ca="1">INDIRECT(ADDRESS(K24+2,24))/(MAX(N24,O24,P24)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1553611240208257</v>
       </c>
-      <c r="S24" s="103">
+      <c r="S24" s="90">
         <v>13.37659</v>
       </c>
     </row>
@@ -3336,7 +3345,7 @@
         <f t="array" aca="1" ref="R25" ca="1">INDIRECT(ADDRESS(K25+2,24))/(MAX(N25,O25,P25)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.5700953344738129</v>
       </c>
-      <c r="S25" s="103">
+      <c r="S25" s="90">
         <v>13.97856</v>
       </c>
     </row>
@@ -3399,7 +3408,7 @@
         <f t="array" aca="1" ref="R26" ca="1">INDIRECT(ADDRESS(K26+2,24))/(MAX(N26,O26,P26)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1820363854567271</v>
       </c>
-      <c r="S26" s="103">
+      <c r="S26" s="90">
         <v>13.76496</v>
       </c>
     </row>
@@ -3462,7 +3471,7 @@
         <f t="array" aca="1" ref="R27" ca="1">INDIRECT(ADDRESS(K27+2,24))/(MAX(N27,O27,P27)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.1874508678027733</v>
       </c>
-      <c r="S27" s="103">
+      <c r="S27" s="90">
         <v>13.813499999999999</v>
       </c>
     </row>
@@ -3525,7 +3534,7 @@
         <f t="array" aca="1" ref="R28" ca="1">INDIRECT(ADDRESS(K28+2,24))/(MAX(N28,O28,P28)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.95464013242686852</v>
       </c>
-      <c r="S28" s="103">
+      <c r="S28" s="90">
         <v>13.17076</v>
       </c>
     </row>
@@ -3588,7 +3597,7 @@
         <f t="array" aca="1" ref="R29" ca="1">INDIRECT(ADDRESS(K29+2,24))/(MAX(N29,O29,P29)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.86767521128075797</v>
       </c>
-      <c r="S29" s="103">
+      <c r="S29" s="90">
         <v>13.182410000000001</v>
       </c>
     </row>
@@ -3651,7 +3660,7 @@
         <f t="array" aca="1" ref="R30" ca="1">INDIRECT(ADDRESS(K30+2,24))/(MAX(N30,O30,P30)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>1.2778881129832498</v>
       </c>
-      <c r="S30" s="103">
+      <c r="S30" s="90">
         <v>13.37659</v>
       </c>
     </row>
@@ -3714,7 +3723,7 @@
         <f t="array" aca="1" ref="R31" ca="1">INDIRECT(ADDRESS(K31+2,24))/(MAX(N31,O31,P31)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.27023443764339738</v>
       </c>
-      <c r="S31" s="103">
+      <c r="S31" s="90">
         <v>11.9008</v>
       </c>
     </row>
@@ -3777,7 +3786,7 @@
         <f t="array" aca="1" ref="R32" ca="1">INDIRECT(ADDRESS(K32+2,24))/(MAX(N32,O32,P32)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.34176971038739401</v>
       </c>
-      <c r="S32" s="103">
+      <c r="S32" s="90">
         <v>11.9979</v>
       </c>
     </row>
@@ -3840,7 +3849,7 @@
         <f t="array" aca="1" ref="R33" ca="1">INDIRECT(ADDRESS(K33+2,24))/(MAX(N33,O33,P33)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.53311773865133549</v>
       </c>
-      <c r="S33" s="103">
+      <c r="S33" s="90">
         <v>12.13382</v>
       </c>
     </row>
@@ -3903,7 +3912,7 @@
         <f t="array" aca="1" ref="R34" ca="1">INDIRECT(ADDRESS(K34+2,24))/(MAX(N34,O34,P34)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.6570351498581164</v>
       </c>
-      <c r="S34" s="103">
+      <c r="S34" s="90">
         <v>12.17266</v>
       </c>
     </row>
@@ -3966,7 +3975,7 @@
         <f t="array" aca="1" ref="R35" ca="1">INDIRECT(ADDRESS(K35+2,24))/(MAX(N35,O35,P35)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.87562276537131445</v>
       </c>
-      <c r="S35" s="103">
+      <c r="S35" s="90">
         <v>12.24062</v>
       </c>
     </row>
@@ -4029,7 +4038,7 @@
         <f t="array" aca="1" ref="R36" ca="1">INDIRECT(ADDRESS(K36+2,24))/(MAX(N36,O36,P36)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.94172400820378366</v>
       </c>
-      <c r="S36" s="103">
+      <c r="S36" s="90">
         <v>11.990130000000001</v>
       </c>
     </row>
@@ -4092,7 +4101,7 @@
         <f t="array" aca="1" ref="R37" ca="1">INDIRECT(ADDRESS(K37+2,24))/(MAX(N37,O37,P37)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.95031570735512783</v>
       </c>
-      <c r="S37" s="103">
+      <c r="S37" s="90">
         <v>11.939640000000001</v>
       </c>
     </row>
@@ -4155,7 +4164,7 @@
         <f t="array" aca="1" ref="R38" ca="1">INDIRECT(ADDRESS(K38+2,24))/(MAX(N38,O38,P38)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.85979472515721045</v>
       </c>
-      <c r="S38" s="103">
+      <c r="S38" s="90">
         <v>11.87168</v>
       </c>
     </row>
@@ -4218,7 +4227,7 @@
         <f t="array" aca="1" ref="R39" ca="1">INDIRECT(ADDRESS(K39+2,24))/(MAX(N39,O39,P39)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.79540264709677744</v>
       </c>
-      <c r="S39" s="103">
+      <c r="S39" s="90">
         <v>11.82799</v>
       </c>
     </row>
@@ -4281,7 +4290,7 @@
         <f t="array" aca="1" ref="R40" ca="1">INDIRECT(ADDRESS(K40+2,24))/(MAX(N40,O40,P40)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.72851509749905463</v>
       </c>
-      <c r="S40" s="103">
+      <c r="S40" s="90">
         <v>11.78429</v>
       </c>
     </row>
@@ -4344,14 +4353,75 @@
         <f t="array" aca="1" ref="R41" ca="1">INDIRECT(ADDRESS(K41+2,24))/(MAX(N41,O41,P41)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
         <v>0.51467817822082118</v>
       </c>
-      <c r="S41" s="103">
+      <c r="S41" s="90">
         <v>11.740600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J42" s="20"/>
+      <c r="K42" s="39"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2.2955E-2</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2.2955E-2</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" s="4">
+        <v>9.1E-4</v>
+      </c>
+      <c r="J43" s="20" t="str" cm="1">
+        <f t="array" aca="1" ref="J43" ca="1">INDIRECT(ADDRESS(K43+2,22))</f>
+        <v>CFRP</v>
+      </c>
+      <c r="K43" s="39">
+        <v>2</v>
+      </c>
+      <c r="L43" s="43">
+        <v>155.04839999999999</v>
+      </c>
+      <c r="M43" s="43">
+        <v>750.14570000000003</v>
+      </c>
+      <c r="N43" s="43">
+        <v>23100000</v>
+      </c>
+      <c r="O43" s="43">
+        <v>27000000</v>
+      </c>
+      <c r="P43" s="43">
+        <v>58000000</v>
+      </c>
+      <c r="Q43" s="21" cm="1">
+        <f t="array" aca="1" ref="Q43" ca="1">INDIRECT(ADDRESS(K43+2,23))/(MAX(N43,O43,P43)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,29))) -1</f>
+        <v>0.61921293297753799</v>
+      </c>
+      <c r="R43" s="22" cm="1">
+        <f t="array" aca="1" ref="R43" ca="1">INDIRECT(ADDRESS(K43+2,24))/(MAX(N43,O43,P43)*INDIRECT(ADDRESS(3,26))*INDIRECT(ADDRESS(3,27))*INDIRECT(ADDRESS(3,28))*INDIRECT(ADDRESS(3,30))) -1</f>
+        <v>0.51990120642158266</v>
+      </c>
+      <c r="S43" s="90">
+        <v>11.920109999999999</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C45" s="101">
-        <v>9.5500000000000001E-4</v>
-      </c>
+      <c r="C45" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4368,32 +4438,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S18 S21:S1048576">
-    <cfRule type="top10" dxfId="13" priority="11" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="12" priority="12" percent="1" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="11" priority="13" rank="4"/>
-    <cfRule type="top10" dxfId="10" priority="14" rank="3"/>
+    <cfRule type="top10" dxfId="3" priority="11" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="2" priority="12" percent="1" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="1" priority="13" rank="4"/>
+    <cfRule type="top10" dxfId="0" priority="14" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19">
-    <cfRule type="top10" dxfId="8" priority="6" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="7" priority="7" percent="1" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="6" priority="8" rank="4"/>
-    <cfRule type="top10" dxfId="5" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="12" priority="6" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="11" priority="7" percent="1" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="10" priority="8" rank="4"/>
+    <cfRule type="top10" dxfId="9" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" bottom="1" rank="4"/>
-    <cfRule type="top10" dxfId="1" priority="3" rank="4"/>
-    <cfRule type="top10" dxfId="0" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="7" priority="1" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="6" priority="2" percent="1" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="5" priority="3" rank="4"/>
+    <cfRule type="top10" dxfId="4" priority="4" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>